<commit_message>
Fix: Strict filtering of core and elective courses
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_DSAI_pre_mid_timetable.xlsx
+++ b/backend/output_timetables/sem1_DSAI_pre_mid_timetable.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CS161 [C205]</t>
+          <t>CS161 [C004]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EC161 [C001]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -548,17 +548,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CS161 [C205]</t>
+          <t>CS161 [L408]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MA161 [C002]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DS161 [C002]</t>
+          <t>DS161 [C104]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -612,17 +612,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L404]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DS161 [C002]</t>
+          <t>DS161 [L407]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MA162 [C001]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L404]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -676,17 +676,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MA161 [C002]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MA162 [C002]</t>
+          <t>MA162 [L405]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>EC161 [C001]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>11.25</v>
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -872,16 +872,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>18.75</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -940,16 +940,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>18.75</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1076,16 +1076,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1348,16 +1348,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1416,16 +1416,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1838,16 +1838,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1906,16 +1906,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -1974,16 +1974,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -2008,16 +2008,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CS161 [C205]</t>
+          <t>CS161 [C004]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EC161 [C001]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2148,17 +2148,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CS161 [C205]</t>
+          <t>CS161 [L408]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MA161 [C002]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DS161 [C002]</t>
+          <t>DS161 [C104]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L403]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DS161 [C002]</t>
+          <t>DS161 [L407]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MA162 [C001]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L403]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2276,17 +2276,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MA161 [C002]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MA162 [C002]</t>
+          <t>MA162 [L405]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>EC161 [C001]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2375,7 +2375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2408,12 +2408,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C004</t>
         </is>
       </c>
     </row>
@@ -2425,12 +2425,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C302</t>
         </is>
       </c>
     </row>
@@ -2442,12 +2442,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS152</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C303</t>
         </is>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C304</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C305</t>
         </is>
       </c>
     </row>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>L402</t>
         </is>
       </c>
     </row>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C102</t>
+          <t>L404</t>
         </is>
       </c>
     </row>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C104</t>
+          <t>L405</t>
         </is>
       </c>
     </row>
@@ -2566,24 +2566,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C202</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>C001, C205</t>
+          <t>L406</t>
         </is>
       </c>
     </row>
@@ -2708,17 +2691,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>introduction to cyber security</t>
+          <t>Problem Solving</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Manjunath</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>3-0-2-0-4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2738,12 +2721,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>L404, C205</t>
+          <t>L207, C004, L408</t>
         </is>
       </c>
     </row>
@@ -2790,7 +2773,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C004</t>
         </is>
       </c>
     </row>
@@ -2837,7 +2820,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C104, L407</t>
         </is>
       </c>
     </row>
@@ -2884,7 +2867,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>C002, C001</t>
+          <t>C004, L405</t>
         </is>
       </c>
     </row>
@@ -2931,7 +2914,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>L105, C001</t>
+          <t>C004, C003, L105</t>
         </is>
       </c>
     </row>
@@ -2948,12 +2931,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Complete: 3</t>
+          <t>Complete: 2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rate: 50.0%</t>
+          <t>Rate: 33.3%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2973,7 +2956,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[WARN] 3 issues</t>
+          <t>[WARN] 4 issues</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -2993,7 +2976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3051,7 +3034,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3061,11 +3044,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Projector</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3073,38 +3061,38 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>MA162, EC161</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.6</t>
+          <t>0.2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>240</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -3116,11 +3104,11 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>MA162, DS161, MA161</t>
+          <t>EC161, CS161, MA162...</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -3132,7 +3120,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3147,11 +3135,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -3163,12 +3151,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.2</t>
         </is>
       </c>
     </row>
@@ -3218,22 +3206,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>L404</t>
+          <t>L207</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>Software Lab</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>40</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Computers</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -3255,6 +3243,135 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>L405</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>L407</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>L408</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.2</t>
         </is>
       </c>
     </row>
@@ -3269,7 +3386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3305,47 +3422,57 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Course</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Room Type</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Capacity</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Conflict</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Allocation Type</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Basket</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>room</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>course</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>session_type</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>conflict</t>
         </is>
       </c>
     </row>
@@ -3375,42 +3502,50 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>C205</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
+          <t>L408</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>CS161</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -3439,42 +3574,50 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>CS161 (Lab)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>Software Lab</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>TV</t>
-        </is>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr">
+          <t>40</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>L403</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
+          <t>L207</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
           <t>CS161 (Lab)</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Lab</t>
         </is>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -3503,42 +3646,50 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>CS161 (Lab)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>Software Lab</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>TV</t>
-        </is>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr">
+          <t>40</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>L403</t>
-        </is>
-      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
+          <t>L207</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
           <t>CS161 (Lab)</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>Lab</t>
         </is>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3567,42 +3718,50 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
           <t>MA161</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3631,42 +3790,50 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>TV</t>
-        </is>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr">
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>C205</t>
-        </is>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
           <t>CS161</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -3695,42 +3862,50 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr">
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
           <t>MA161</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -3759,42 +3934,50 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
+          <t>L407</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3823,42 +4006,50 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
+          <t>L405</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
           <t>MA162</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -3887,42 +4078,50 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>Projector</t>
         </is>
       </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
+          <t>C104</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -3951,38 +4150,50 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="inlineStr">
+          <t>Auditorium</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
-      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
           <t>MA162</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -4011,38 +4222,50 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
+          <t>Auditorium</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
-      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -4071,38 +4294,50 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>large classroom</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" t="inlineStr">
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
+          <t>C003</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -4131,42 +4366,50 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>EC161 (Lab)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Hardware Lab</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Equipment</t>
         </is>
       </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
         <is>
           <t>L105</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>EC161 (Lab)</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>Lab</t>
         </is>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -4195,42 +4438,50 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>EC161 (Lab)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Hardware Lab</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Equipment</t>
         </is>
       </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>Global Tracking</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
         <is>
           <t>L105</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>EC161 (Lab)</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>Lab</t>
         </is>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -4259,46 +4510,54 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>TV</t>
-        </is>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="inlineStr">
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>C203</t>
-        </is>
-      </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -4327,46 +4586,54 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="inlineStr">
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -4395,46 +4662,54 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>HS152</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="inlineStr">
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>C003</t>
-        </is>
-      </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -4463,46 +4738,54 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>96</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="inlineStr">
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>C202</t>
-        </is>
-      </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -4531,46 +4814,54 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>96</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>C204</t>
-        </is>
-      </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>C305</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -4599,46 +4890,54 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>large classroom</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>Projector</t>
         </is>
       </c>
-      <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" t="inlineStr">
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -4667,46 +4966,54 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>C102</t>
-        </is>
-      </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>HS103</t>
+          <t>L402</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -4735,46 +5042,54 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>C104</t>
-        </is>
-      </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>DE101</t>
+          <t>L404</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -4803,46 +5118,54 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I24" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>C101</t>
-        </is>
-      </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>L405</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -4871,46 +5194,54 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>C302</t>
-        </is>
-      </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -4929,7 +5260,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -4939,42 +5270,54 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" t="inlineStr">
+          <t>Auditorium</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
-      </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -4993,45 +5336,65 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>13:00-14:30</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" t="inlineStr">
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>DS161</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr"/>
+          <t>C302</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Lecture</t>
+        </is>
+      </c>
+      <c r="P27" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -5059,46 +5422,54 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>96</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="I28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J28" t="inlineStr">
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>C203</t>
-        </is>
-      </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -5127,46 +5498,54 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J29" t="inlineStr">
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -5195,46 +5574,54 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>DS151</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J30" t="inlineStr">
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>C003</t>
-        </is>
-      </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>C305</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -5263,46 +5650,54 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
           <t>Projector</t>
         </is>
       </c>
-      <c r="I31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J31" t="inlineStr">
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="L31" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>C202</t>
-        </is>
-      </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -5331,46 +5726,54 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H32" t="inlineStr">
         <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" t="inlineStr">
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>C204</t>
-        </is>
-      </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>L402</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P32" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -5399,46 +5802,54 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>HS103</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I33" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>L404</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P33" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -5467,46 +5878,54 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I34" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>C102</t>
-        </is>
-      </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>HS103</t>
+          <t>L405</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P34" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -5535,46 +5954,54 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I35" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>C104</t>
-        </is>
-      </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>DE101</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
           <t>Lecture</t>
         </is>
+      </c>
+      <c r="P35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -5593,56 +6020,64 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J36" t="inlineStr">
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>C101</t>
-        </is>
-      </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Lecture</t>
-        </is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
+        </is>
+      </c>
+      <c r="P36" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -5661,56 +6096,64 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>96</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>Projector</t>
         </is>
       </c>
-      <c r="I37" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" t="inlineStr">
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
+      <c r="M37" t="inlineStr">
         <is>
           <t>C302</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>HS152</t>
-        </is>
-      </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Lecture</t>
-        </is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
+        </is>
+      </c>
+      <c r="P37" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -5729,52 +6172,64 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>HS152</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" t="inlineStr">
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
+      <c r="L38" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
-      </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Lecture</t>
-        </is>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
+        </is>
+      </c>
+      <c r="P38" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -5793,7 +6248,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -5803,39 +6258,55 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Hardware Lab</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Equipment</t>
-        </is>
-      </c>
-      <c r="I39" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" t="inlineStr">
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>L206</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr"/>
+          <t>C304</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
+        </is>
+      </c>
+      <c r="P39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -5863,46 +6334,54 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>96</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="I40" t="b">
-        <v>0</v>
-      </c>
-      <c r="J40" t="inlineStr">
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>C203</t>
-        </is>
-      </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>C305</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
           <t>Tutorial</t>
         </is>
+      </c>
+      <c r="P40" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -5931,46 +6410,54 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I41" t="b">
-        <v>0</v>
-      </c>
-      <c r="J41" t="inlineStr">
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
           <t>Tutorial</t>
         </is>
+      </c>
+      <c r="P41" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -5999,46 +6486,54 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>HS102</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
+      <c r="L42" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>C003</t>
-        </is>
-      </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>L402</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
           <t>Tutorial</t>
         </is>
+      </c>
+      <c r="P42" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -6067,46 +6562,54 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I43" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="L43" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>C202</t>
-        </is>
-      </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>L404</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
           <t>Tutorial</t>
         </is>
+      </c>
+      <c r="P43" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -6135,46 +6638,54 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
       <c r="H44" t="inlineStr">
         <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="I44" t="b">
-        <v>0</v>
-      </c>
-      <c r="J44" t="inlineStr">
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>C204</t>
-        </is>
-      </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>L405</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
           <t>Tutorial</t>
         </is>
+      </c>
+      <c r="P44" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -6203,382 +6714,54 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" t="inlineStr">
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>ELECTIVE_B1</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
           <t>Tutorial</t>
         </is>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>1</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>classroom</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I46" t="b">
-        <v>0</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>C102</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Tutorial</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>1</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>classroom</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>C104</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>Tutorial</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>1</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>classroom</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I48" t="b">
-        <v>0</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>C101</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>HS156</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>Tutorial</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>1</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>classroom</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I49" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>C302</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>HS152</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>Tutorial</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>1</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>large classroom</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>Tutorial</t>
-        </is>
+      <c r="P45" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6665,17 +6848,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>introduction to cyber security</t>
+          <t>Problem Solving</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>3-0-2-0-4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2/0/0</t>
+          <t>3/0/2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -6700,7 +6883,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>[FAIL]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -7073,7 +7256,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-01-19 23:36</t>
+          <t>2026-01-26 01:05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -7098,7 +7281,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Core: 4, Elective: 2</t>
+          <t>Core: 5, Elective: 1</t>
         </is>
       </c>
     </row>
@@ -7137,12 +7320,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5/36</t>
+          <t>8/36</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Utilization: 13.9%</t>
+          <t>Utilization: 22.2%</t>
         </is>
       </c>
     </row>
@@ -7201,7 +7384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8294,6 +8477,78 @@
         </is>
       </c>
       <c r="P15" t="inlineStr">
+        <is>
+          <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Girish Revadigar</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
         <is>
           <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
         </is>
@@ -8388,11 +8643,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HS152, HS157, HS156, PH151, DS151, CS101, HS102, HS103, DE101</t>
+          <t>HS157, HS156, HS152, PH151, DS151, CS101, HS102, HS103, DE101, CS151</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -8421,7 +8676,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8474,7 +8729,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -8488,7 +8743,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -8509,7 +8764,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -8523,7 +8778,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -8544,7 +8799,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS152</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -8558,7 +8813,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -8593,7 +8848,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -8628,7 +8883,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -8663,7 +8918,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -8698,7 +8953,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -8733,7 +8988,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -8768,7 +9023,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -8776,6 +9031,41 @@
         </is>
       </c>
       <c r="G10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>